<commit_message>
Ubah Email, Ubah Kata Sandi
</commit_message>
<xml_diff>
--- a/Ubah Kata - Sandi - ATS-22.xlsx
+++ b/Ubah Kata - Sandi - ATS-22.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lieto\git\ACC-Seamless-ACCOne\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lieto\git\ACC-ACCOne\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,6 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="18">
   <si>
     <t>oldPassword</t>
   </si>
@@ -74,16 +75,10 @@
     <t>newPasswordWrong</t>
   </si>
   <si>
-    <t>Application11</t>
-  </si>
-  <si>
-    <t>App1!</t>
-  </si>
-  <si>
-    <t>newPasswordShort</t>
-  </si>
-  <si>
     <t>success</t>
+  </si>
+  <si>
+    <t>Password1!</t>
   </si>
 </sst>
 </file>
@@ -401,10 +396,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -500,7 +495,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>17</v>
@@ -509,21 +504,7 @@
         <v>17</v>
       </c>
       <c r="D8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>